<commit_message>
added pressures and temps
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14664" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16292" uniqueCount="228">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -669,6 +669,36 @@
   </si>
   <si>
     <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUEL T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OIL</t>
   </si>
 </sst>
 </file>
@@ -2788,7 +2818,7 @@
         <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F34" t="s">
         <v>58</v>
@@ -2958,7 +2988,7 @@
         <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F44" t="s">
         <v>58</v>
@@ -3043,7 +3073,7 @@
         <v>80</v>
       </c>
       <c r="E49" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F49" t="s">
         <v>58</v>
@@ -3051,7 +3081,7 @@
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C50" t="s">
         <v>40</v>
@@ -3068,7 +3098,7 @@
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C51" t="s">
         <v>40</v>
@@ -3085,7 +3115,7 @@
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C52" t="s">
         <v>40</v>
@@ -3102,7 +3132,7 @@
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C53" t="s">
         <v>40</v>
@@ -3119,16 +3149,16 @@
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="D54" t="s">
         <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="F54" t="s">
         <v>58</v>
@@ -3136,10 +3166,10 @@
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="D55" t="s">
         <v>80</v>
@@ -3153,16 +3183,16 @@
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C56" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
       </c>
       <c r="E56" t="s">
-        <v>156</v>
+        <v>81</v>
       </c>
       <c r="F56" t="s">
         <v>58</v>
@@ -3170,10 +3200,10 @@
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D57" t="s">
         <v>80</v>
@@ -3187,16 +3217,16 @@
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C58" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="D58" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E58" t="s">
-        <v>81</v>
+        <v>217</v>
       </c>
       <c r="F58" t="s">
         <v>58</v>
@@ -3204,16 +3234,16 @@
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D59" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>215</v>
+        <v>81</v>
       </c>
       <c r="F59" t="s">
         <v>58</v>
@@ -3221,24 +3251,91 @@
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="D60" t="s">
         <v>80</v>
       </c>
       <c r="E60" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" t="s">
+        <v>221</v>
+      </c>
+      <c r="F61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>222</v>
+      </c>
+      <c r="C62" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" t="s">
+        <v>223</v>
+      </c>
+      <c r="F62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>224</v>
+      </c>
+      <c r="C63" t="s">
+        <v>51</v>
+      </c>
+      <c r="D63" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" t="s">
+        <v>225</v>
+      </c>
+      <c r="F63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>226</v>
+      </c>
+      <c r="C64" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" t="s">
+        <v>227</v>
+      </c>
+      <c r="F64" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65"/>
+    <row r="66"/>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added min oil pressure + rearrangement
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16292" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16709" uniqueCount="230">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -699,6 +699,12 @@
   </si>
   <si>
     <t xml:space="preserve">OIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId98</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +1953,9 @@
         <v>4</v>
       </c>
       <c r="F4"/>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
       <c r="H4"/>
       <c r="I4" t="s">
         <v>44</v>
@@ -3152,7 +3160,7 @@
         <v>209</v>
       </c>
       <c r="C54" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D54" t="s">
         <v>57</v>
@@ -3169,7 +3177,7 @@
         <v>210</v>
       </c>
       <c r="C55" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D55" t="s">
         <v>80</v>
@@ -3334,8 +3342,40 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65"/>
-    <row r="66"/>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>228</v>
+      </c>
+      <c r="C65" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" t="s">
+        <v>57</v>
+      </c>
+      <c r="E65" t="s">
+        <v>81</v>
+      </c>
+      <c r="F65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>229</v>
+      </c>
+      <c r="C66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" t="s">
+        <v>217</v>
+      </c>
+      <c r="F66" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>